<commit_message>
gives infos about specific user
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qwerty\Desktop\AllOfTheLaptop\Web0RoniRizk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF96DA4A-EBB9-4645-9B35-3078D471DF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E68FFB-6FB1-4D55-9700-D23263DD698D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -33,86 +33,89 @@
     <t>name</t>
   </si>
   <si>
-    <t>student1</t>
-  </si>
-  <si>
-    <t>student2</t>
-  </si>
-  <si>
-    <t>student3</t>
-  </si>
-  <si>
-    <t>student4</t>
-  </si>
-  <si>
-    <t>student5</t>
-  </si>
-  <si>
-    <t>student6</t>
-  </si>
-  <si>
-    <t>student7</t>
-  </si>
-  <si>
-    <t>student8</t>
-  </si>
-  <si>
-    <t>student9</t>
-  </si>
-  <si>
-    <t>student10</t>
-  </si>
-  <si>
-    <t>student11</t>
-  </si>
-  <si>
-    <t>student12</t>
-  </si>
-  <si>
-    <t>student13</t>
-  </si>
-  <si>
-    <t>student14</t>
-  </si>
-  <si>
-    <t>student15</t>
-  </si>
-  <si>
-    <t>student16</t>
-  </si>
-  <si>
-    <t>student17</t>
-  </si>
-  <si>
-    <t>student18</t>
-  </si>
-  <si>
-    <t>student19</t>
-  </si>
-  <si>
-    <t>student20</t>
-  </si>
-  <si>
-    <t>student21</t>
-  </si>
-  <si>
-    <t>student22</t>
-  </si>
-  <si>
-    <t>student23</t>
-  </si>
-  <si>
-    <t>student24</t>
-  </si>
-  <si>
-    <t>student25</t>
+    <t>Elio</t>
+  </si>
+  <si>
+    <t>Maroun</t>
+  </si>
+  <si>
+    <t>Dania</t>
+  </si>
+  <si>
+    <t>Rita</t>
+  </si>
+  <si>
+    <t>Roni</t>
+  </si>
+  <si>
+    <t>Samir</t>
+  </si>
+  <si>
+    <t>Nada</t>
+  </si>
+  <si>
+    <t>Elissa</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Darine</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Charbel</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>elio@example.com</t>
+  </si>
+  <si>
+    <t>maroun@example.com</t>
+  </si>
+  <si>
+    <t>dania@example.com</t>
+  </si>
+  <si>
+    <t>rita@example.com</t>
+  </si>
+  <si>
+    <t>roni@example.com</t>
+  </si>
+  <si>
+    <t>samir@example.com</t>
+  </si>
+  <si>
+    <t>nada@example.com</t>
+  </si>
+  <si>
+    <t>elissa@example.com</t>
+  </si>
+  <si>
+    <t>jane@example.com</t>
+  </si>
+  <si>
+    <t>darine@example.com</t>
+  </si>
+  <si>
+    <t>chris@example.com</t>
+  </si>
+  <si>
+    <t>charbel@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +125,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,8 +158,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,222 +446,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
+    <col min="4" max="4" width="30.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="C2" s="2">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="C3" s="2">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="C4" s="2">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="C5" s="2">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="C6" s="2">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="C7" s="2">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="C8" s="2">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="C9" s="2">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="C10" s="2">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="C11" s="2">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="C12" s="2">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
+      <c r="C13" s="2">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>